<commit_message>
construcción de tablas descriptivas
</commit_message>
<xml_diff>
--- a/Output/conteos/freq_variables.xlsx
+++ b/Output/conteos/freq_variables.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">var</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t xml:space="preserve">Edad</t>
-  </si>
-  <si>
-    <t xml:space="preserve"/>
   </si>
   <si>
     <t xml:space="preserve">1er NIVEL</t>
@@ -569,19 +566,19 @@
         <v>15</v>
       </c>
       <c r="B8" t="n">
-        <v>90</v>
+        <v>1310</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0107168373422243</v>
+        <v>0.155989521314599</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>585</v>
       </c>
       <c r="F8" t="n">
-        <v>0.000057696745903531</v>
+        <v>0.0337525963535657</v>
       </c>
       <c r="G8" t="s">
         <v>9</v>
@@ -592,19 +589,19 @@
         <v>16</v>
       </c>
       <c r="B9" t="n">
-        <v>1310</v>
+        <v>763</v>
       </c>
       <c r="C9" t="n">
-        <v>0.155989521314599</v>
+        <v>0.0908549654679686</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
       </c>
       <c r="E9" t="n">
-        <v>585</v>
+        <v>13457</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0337525963535657</v>
+        <v>0.776425109623817</v>
       </c>
       <c r="G9" t="s">
         <v>9</v>
@@ -615,19 +612,19 @@
         <v>17</v>
       </c>
       <c r="B10" t="n">
-        <v>763</v>
+        <v>6232</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0908549654679686</v>
+        <v>0.742081447963801</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
       </c>
       <c r="E10" t="n">
-        <v>13457</v>
+        <v>3289</v>
       </c>
       <c r="F10" t="n">
-        <v>0.776425109623817</v>
+        <v>0.189764597276714</v>
       </c>
       <c r="G10" t="s">
         <v>9</v>
@@ -638,40 +635,38 @@
         <v>18</v>
       </c>
       <c r="B11" t="n">
-        <v>6232</v>
+        <v>3</v>
       </c>
       <c r="C11" t="n">
-        <v>0.742081447963801</v>
+        <v>0.000357227911407478</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
       </c>
-      <c r="E11" t="n">
-        <v>3289</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.189764597276714</v>
-      </c>
-      <c r="G11" t="s">
-        <v>9</v>
-      </c>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
     </row>
     <row r="12">
-      <c r="A12" t="s">
-        <v>19</v>
-      </c>
+      <c r="A12"/>
       <c r="B12" t="n">
-        <v>3</v>
+        <v>90</v>
       </c>
       <c r="C12" t="n">
-        <v>0.000357227911407478</v>
+        <v>0.0107168373422243</v>
       </c>
       <c r="D12" t="s">
         <v>9</v>
       </c>
-      <c r="E12"/>
-      <c r="F12"/>
-      <c r="G12"/>
+      <c r="E12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.000057696745903531</v>
+      </c>
+      <c r="G12" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>